<commit_message>
Ændrer i syssetting p5 for at tjekke results  i 2013
</commit_message>
<xml_diff>
--- a/TIMES-DE/SysSettings.xlsx
+++ b/TIMES-DE/SysSettings.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17016" windowHeight="10416" tabRatio="853" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17016" windowHeight="10416" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -4751,8 +4751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4851,7 +4851,7 @@
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="9">
         <v>1</v>
@@ -4871,7 +4871,7 @@
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="9">
         <v>1</v>
@@ -5817,7 +5817,7 @@
   </sheetPr>
   <dimension ref="A3:BH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Degree of Electrification TRA
</commit_message>
<xml_diff>
--- a/TIMES-DE/SysSettings.xlsx
+++ b/TIMES-DE/SysSettings.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E6E49E-A5CF-4139-8AAC-20AF3F2672B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="853" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="853" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -25,7 +19,7 @@
   <definedNames>
     <definedName name="VEDA2">'Import Settings'!$C$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Maurizio Gargiulo</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,12 +59,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Antti L</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -89,12 +83,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Antti L</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -112,14 +106,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -134,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="1016">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -3179,12 +3173,15 @@
   </si>
   <si>
     <t>https://www.csilmilano.com/docs/WP2013_03.pdf</t>
+  </si>
+  <si>
+    <t>P10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_([$€]* #,##0.00_);_([$€]* \(#,##0.00\);_([$€]* &quot;-&quot;??_);_(@_)"/>
@@ -3786,7 +3783,7 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -4026,31 +4023,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="5x indented GHG Textfiels" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="AggOrange_CRFReport-template" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="AggOrange9_CRFReport-template" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="CustomizationCells" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Euro" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="InputCells" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="5x indented GHG Textfiels" xfId="1"/>
+    <cellStyle name="AggOrange_CRFReport-template" xfId="2"/>
+    <cellStyle name="AggOrange9_CRFReport-template" xfId="3"/>
+    <cellStyle name="CustomizationCells" xfId="4"/>
+    <cellStyle name="Euro" xfId="5"/>
+    <cellStyle name="InputCells" xfId="6"/>
     <cellStyle name="Link" xfId="20" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Normal 10 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Normal 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Normal 3" xfId="10" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Normal 4" xfId="11" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Normal GHG Numbers (0.00)" xfId="12" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Normal GHG Textfiels Bold" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Normal GHG-Shade" xfId="14" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Normale_B2020" xfId="15" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 10" xfId="7"/>
+    <cellStyle name="Normal 10 2" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="10"/>
+    <cellStyle name="Normal 4" xfId="11"/>
+    <cellStyle name="Normal GHG Numbers (0.00)" xfId="12"/>
+    <cellStyle name="Normal GHG Textfiels Bold" xfId="13"/>
+    <cellStyle name="Normal GHG-Shade" xfId="14"/>
+    <cellStyle name="Normale_B2020" xfId="15"/>
     <cellStyle name="Procent" xfId="16" builtinId="5"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Standaard_Blad1" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Обычный_CRF2002 (1)" xfId="18" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="17"/>
+    <cellStyle name="Standaard_Blad1" xfId="19"/>
+    <cellStyle name="Обычный_CRF2002 (1)" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4085,7 +4083,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9563E5EE-A894-47F4-BFC6-EAD796C87904}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9563E5EE-A894-47F4-BFC6-EAD796C87904}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4115,9 +4113,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kontortema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4155,9 +4153,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4190,26 +4188,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4242,26 +4223,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4434,7 +4398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
@@ -4444,17 +4408,17 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.08984375" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.08984375" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="7" t="s">
         <v>6</v>
@@ -4465,7 +4429,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
@@ -4483,7 +4447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="67" t="s">
         <v>1007</v>
       </c>
@@ -4520,7 +4484,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="67"/>
       <c r="C6" s="68" t="s">
         <v>1009</v>
@@ -4555,7 +4519,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="67"/>
       <c r="C7" s="68" t="s">
@@ -4582,7 +4546,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="67"/>
       <c r="C8" s="68" t="s">
@@ -4609,7 +4573,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="68"/>
       <c r="C9" s="68" t="s">
@@ -4626,7 +4590,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="67"/>
       <c r="C10" s="68"/>
@@ -4640,7 +4604,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="67"/>
       <c r="C11" s="68"/>
@@ -4654,7 +4618,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="67"/>
       <c r="C12" s="68"/>
@@ -4662,7 +4626,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4670,7 +4634,7 @@
       <c r="O13" s="13"/>
       <c r="P13" s="14"/>
     </row>
-    <row r="14" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4678,7 +4642,7 @@
       <c r="O14" s="13"/>
       <c r="P14" s="14"/>
     </row>
-    <row r="15" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="114"/>
       <c r="C15" s="3"/>
@@ -4686,90 +4650,90 @@
       <c r="O15" s="13"/>
       <c r="P15" s="14"/>
     </row>
-    <row r="16" spans="1:18" ht="13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="115"/>
       <c r="C16" s="115"/>
       <c r="O16" s="13"/>
       <c r="P16" s="14"/>
     </row>
-    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="115"/>
       <c r="C17" s="115"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="115"/>
       <c r="C18" s="115"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="115"/>
       <c r="C19" s="115"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
     </row>
   </sheetData>
@@ -4783,32 +4747,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K57"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>32</v>
       </c>
@@ -4819,7 +4783,7 @@
       <c r="I7" s="69"/>
       <c r="J7" s="69"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -4828,23 +4792,23 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="71" t="str">
         <f ca="1">IF(VEDA2,"~DefaultYear",T(0))</f>
         <v>~DefaultYear</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="70">
         <v>2010</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="64" t="s">
         <v>44</v>
       </c>
@@ -4854,6 +4818,9 @@
       <c r="D16" s="65" t="s">
         <v>1006</v>
       </c>
+      <c r="E16" s="149" t="s">
+        <v>1015</v>
+      </c>
       <c r="I16" s="149" t="s">
         <v>44</v>
       </c>
@@ -4864,7 +4831,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="9">
         <v>1</v>
       </c>
@@ -4874,6 +4841,9 @@
       <c r="D17" s="9">
         <v>1</v>
       </c>
+      <c r="E17" s="9">
+        <v>1</v>
+      </c>
       <c r="I17">
         <v>2010</v>
       </c>
@@ -4884,7 +4854,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="9">
         <v>3</v>
       </c>
@@ -4894,6 +4864,9 @@
       <c r="D18" s="9">
         <v>1</v>
       </c>
+      <c r="E18" s="9">
+        <v>3</v>
+      </c>
       <c r="I18">
         <v>2013</v>
       </c>
@@ -4904,7 +4877,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="9">
         <v>4</v>
       </c>
@@ -4914,6 +4887,9 @@
       <c r="D19" s="9">
         <v>1</v>
       </c>
+      <c r="E19" s="9">
+        <v>4</v>
+      </c>
       <c r="I19">
         <v>2015</v>
       </c>
@@ -4924,7 +4900,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="9">
         <v>5</v>
       </c>
@@ -4934,6 +4910,9 @@
       <c r="D20" s="9">
         <v>1</v>
       </c>
+      <c r="E20" s="151">
+        <v>5</v>
+      </c>
       <c r="I20">
         <v>2020</v>
       </c>
@@ -4944,7 +4923,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="9">
         <v>5</v>
       </c>
@@ -4954,6 +4933,9 @@
       <c r="D21" s="9">
         <v>1</v>
       </c>
+      <c r="E21" s="151">
+        <v>5</v>
+      </c>
       <c r="I21">
         <v>2025</v>
       </c>
@@ -4964,7 +4946,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="9">
         <v>5</v>
       </c>
@@ -4974,6 +4956,9 @@
       <c r="D22" s="9">
         <v>1</v>
       </c>
+      <c r="E22" s="151">
+        <v>10</v>
+      </c>
       <c r="I22">
         <v>2030</v>
       </c>
@@ -4984,7 +4969,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="9">
         <v>5</v>
       </c>
@@ -4994,6 +4979,9 @@
       <c r="D23" s="9">
         <v>1</v>
       </c>
+      <c r="E23" s="151">
+        <v>10</v>
+      </c>
       <c r="I23">
         <v>2035</v>
       </c>
@@ -5004,7 +4992,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="9">
         <v>5</v>
       </c>
@@ -5014,6 +5002,9 @@
       <c r="D24" s="9">
         <v>1</v>
       </c>
+      <c r="E24" s="151">
+        <v>10</v>
+      </c>
       <c r="I24">
         <v>2040</v>
       </c>
@@ -5024,7 +5015,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="9">
         <v>5</v>
       </c>
@@ -5044,7 +5035,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="9">
         <v>5</v>
       </c>
@@ -5064,7 +5055,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="9">
         <v>15</v>
       </c>
@@ -5084,7 +5075,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="9">
         <v>1</v>
@@ -5099,7 +5090,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C29" s="9">
         <v>1</v>
       </c>
@@ -5113,7 +5104,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C30" s="9">
         <v>1</v>
       </c>
@@ -5127,7 +5118,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C31" s="9">
         <v>1</v>
       </c>
@@ -5141,7 +5132,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C32" s="9">
         <v>1</v>
       </c>
@@ -5155,7 +5146,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" s="9">
         <v>1</v>
       </c>
@@ -5169,7 +5160,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" s="9">
         <v>1</v>
       </c>
@@ -5183,7 +5174,7 @@
         <v>2027</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="9">
         <v>1</v>
       </c>
@@ -5197,7 +5188,7 @@
         <v>2028</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C36" s="9">
         <v>1</v>
       </c>
@@ -5211,7 +5202,7 @@
         <v>2029</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" s="9">
         <v>1</v>
       </c>
@@ -5225,7 +5216,7 @@
         <v>2030</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C38" s="9">
         <v>1</v>
       </c>
@@ -5239,7 +5230,7 @@
         <v>2031</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C39" s="9">
         <v>1</v>
       </c>
@@ -5253,7 +5244,7 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C40" s="9">
         <v>1</v>
       </c>
@@ -5267,7 +5258,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C41" s="9">
         <v>1</v>
       </c>
@@ -5281,7 +5272,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C42" s="9">
         <v>1</v>
       </c>
@@ -5295,7 +5286,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" s="9">
         <v>1</v>
       </c>
@@ -5309,7 +5300,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C44" s="9">
         <v>1</v>
       </c>
@@ -5318,7 +5309,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C45" s="9">
         <v>1</v>
       </c>
@@ -5327,7 +5318,7 @@
         <v>2038</v>
       </c>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C46" s="9">
         <v>1</v>
       </c>
@@ -5336,7 +5327,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" s="9">
         <v>1</v>
       </c>
@@ -5345,7 +5336,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C48" s="9">
         <v>1</v>
       </c>
@@ -5354,7 +5345,7 @@
         <v>2041</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C49" s="9">
         <v>1</v>
       </c>
@@ -5363,7 +5354,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C50" s="9">
         <v>1</v>
       </c>
@@ -5372,7 +5363,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C51" s="9">
         <v>1</v>
       </c>
@@ -5381,7 +5372,7 @@
         <v>2044</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="9">
         <v>1</v>
       </c>
@@ -5390,7 +5381,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C53" s="9">
         <v>1</v>
       </c>
@@ -5399,7 +5390,7 @@
         <v>2046</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C54" s="9">
         <v>1</v>
       </c>
@@ -5408,7 +5399,7 @@
         <v>2047</v>
       </c>
     </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C55" s="9">
         <v>1</v>
       </c>
@@ -5417,7 +5408,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C56" s="9">
         <v>1</v>
       </c>
@@ -5426,7 +5417,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C57" s="9">
         <v>1</v>
       </c>
@@ -5445,47 +5436,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X28"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="13" width="8" customWidth="1"/>
-    <col min="17" max="17" width="21.453125" customWidth="1"/>
-    <col min="18" max="18" width="15.54296875" customWidth="1"/>
-    <col min="20" max="20" width="7.54296875" customWidth="1"/>
-    <col min="21" max="21" width="8.08984375" customWidth="1"/>
+    <col min="17" max="17" width="21.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" customWidth="1"/>
     <col min="22" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="str">
         <f ca="1">IF(VEDA2,"~TFM_MIG","~TFM_UPD")</f>
         <v>~TFM_MIG</v>
       </c>
     </row>
-    <row r="6" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -5529,7 +5520,7 @@
       <c r="W6" s="8"/>
       <c r="X6" s="8"/>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B7" s="77" t="s">
         <v>23</v>
       </c>
@@ -5572,7 +5563,7 @@
       <c r="W7" s="67"/>
       <c r="X7" s="67"/>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B8" s="69"/>
       <c r="C8" s="69" t="s">
         <v>67</v>
@@ -5613,30 +5604,30 @@
       <c r="W8" s="67"/>
       <c r="X8" s="67"/>
     </row>
-    <row r="11" spans="2:24" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="2:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="2:24" ht="13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
@@ -5650,7 +5641,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="69" t="s">
         <v>4</v>
       </c>
@@ -5664,7 +5655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="69" t="s">
         <v>4</v>
       </c>
@@ -5679,19 +5670,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:13" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>951</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="2:13" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:13" ht="18" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -5699,12 +5690,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="26" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>17</v>
       </c>
@@ -5722,7 +5713,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="77" t="s">
         <v>947</v>
       </c>
@@ -5737,7 +5728,7 @@
       </c>
       <c r="F27" s="69"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="77"/>
       <c r="C28" s="69" t="s">
         <v>960</v>
@@ -5760,23 +5751,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B1" s="17" t="str">
         <f ca="1">"~Scenario:"&amp;REPLACE(REPLACE($F$1,FIND(".",$F$1),100,""),1,FIND("[",$F$1),"")</f>
-        <v>~Scenario:SysSettings</v>
+        <v>~Scenario:</v>
       </c>
       <c r="C1" s="34" t="b">
         <f ca="1">NOT(ISERR(FIND(".xlsx",$F$1)))</f>
@@ -5787,17 +5778,17 @@
       </c>
       <c r="F1" s="17" t="str">
         <f ca="1">CELL("filename",$E$1)</f>
-        <v>C:\Users\Julius Steensberg\OneDrive\Desktop\GitHub\Bachelor_Git\TIMES-DE\[SysSettings.xlsx]Import Settings</v>
+        <v>C:\Users\hjs.MEDICOUH\Documents\GitHub\Bachelor_Git\TIMES-DE\[SysSettings.xlsx]Import Settings</v>
       </c>
       <c r="I1" s="66"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="3" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="18" t="s">
         <v>25</v>
       </c>
@@ -5805,7 +5796,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="15" t="s">
         <v>27</v>
       </c>
@@ -5813,7 +5804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
         <v>28</v>
       </c>
@@ -5821,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
@@ -5829,7 +5820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
         <v>30</v>
       </c>
@@ -5837,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>62</v>
       </c>
@@ -5854,40 +5845,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
   <dimension ref="A3:BH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.453125" style="56" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" style="56" customWidth="1"/>
-    <col min="3" max="3" width="12.36328125" style="56" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" style="56" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.90625" style="56" customWidth="1"/>
-    <col min="6" max="10" width="8.36328125" style="56" customWidth="1"/>
-    <col min="11" max="15" width="9.08984375" style="56"/>
-    <col min="16" max="16" width="18.6328125" style="56" customWidth="1"/>
-    <col min="17" max="16384" width="9.08984375" style="56"/>
+    <col min="1" max="1" width="3.42578125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="56" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="56" customWidth="1"/>
+    <col min="6" max="10" width="8.42578125" style="56" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="56"/>
+    <col min="16" max="16" width="18.5703125" style="56" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="56"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:57" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:57" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:57" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:57" x14ac:dyDescent="0.2">
       <c r="B5" s="94" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:57" ht="26" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:57" ht="25.5" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -5967,7 +5958,7 @@
       <c r="BD6"/>
       <c r="BE6"/>
     </row>
-    <row r="7" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="99"/>
       <c r="C7" s="99" t="s">
         <v>49</v>
@@ -6031,7 +6022,7 @@
       <c r="BD7"/>
       <c r="BE7"/>
     </row>
-    <row r="8" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="100"/>
       <c r="C8" s="100" t="s">
         <v>35</v>
@@ -6101,7 +6092,7 @@
       <c r="BD8"/>
       <c r="BE8"/>
     </row>
-    <row r="9" spans="2:57" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:57" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="104"/>
       <c r="C9" s="67" t="s">
         <v>78</v>
@@ -6173,7 +6164,7 @@
       <c r="BD9"/>
       <c r="BE9"/>
     </row>
-    <row r="10" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="104"/>
       <c r="C10" s="67" t="s">
         <v>78</v>
@@ -6322,7 +6313,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="104"/>
       <c r="C11" s="67" t="s">
         <v>78</v>
@@ -6513,7 +6504,7 @@
         <v>3.1586828119702575</v>
       </c>
     </row>
-    <row r="12" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="104"/>
       <c r="C12" s="67" t="s">
         <v>78</v>
@@ -6705,7 +6696,7 @@
         <v>1.8113615841033557</v>
       </c>
     </row>
-    <row r="13" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="104"/>
       <c r="C13" s="67" t="s">
         <v>78</v>
@@ -6857,7 +6848,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="104"/>
       <c r="C14" s="67" t="s">
         <v>78</v>
@@ -7050,7 +7041,7 @@
         <v>3.5169849357346781</v>
       </c>
     </row>
-    <row r="15" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="104"/>
       <c r="C15" s="67" t="s">
         <v>78</v>
@@ -7243,7 +7234,7 @@
         <v>0.24313578310112163</v>
       </c>
     </row>
-    <row r="16" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:57" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="104"/>
       <c r="C16" s="67" t="s">
         <v>78</v>
@@ -7435,7 +7426,7 @@
         <v>0.19507769807358924</v>
       </c>
     </row>
-    <row r="17" spans="1:60" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:60" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="104"/>
       <c r="C17" s="67" t="s">
         <v>78</v>
@@ -7627,7 +7618,7 @@
         <v>1.9126558372437869E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="104"/>
       <c r="C18" s="67" t="s">
         <v>78</v>
@@ -7694,7 +7685,7 @@
       <c r="BD18"/>
       <c r="BE18"/>
     </row>
-    <row r="19" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="99"/>
       <c r="C19" s="67" t="s">
         <v>78</v>
@@ -7761,7 +7752,7 @@
       <c r="BD19"/>
       <c r="BE19"/>
     </row>
-    <row r="20" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="99"/>
       <c r="C20" s="67" t="s">
         <v>78</v>
@@ -7829,7 +7820,7 @@
       <c r="BD20"/>
       <c r="BE20"/>
     </row>
-    <row r="21" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="99"/>
       <c r="C21" s="67" t="s">
         <v>78</v>
@@ -7901,7 +7892,7 @@
       <c r="BD21"/>
       <c r="BE21"/>
     </row>
-    <row r="22" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="99"/>
       <c r="C22" s="67" t="s">
         <v>78</v>
@@ -7967,7 +7958,7 @@
       <c r="BD22" s="30"/>
       <c r="BE22"/>
     </row>
-    <row r="23" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="104"/>
       <c r="C23" s="105" t="s">
         <v>78</v>
@@ -7994,7 +7985,7 @@
       <c r="Q23" s="39"/>
       <c r="R23" s="39"/>
     </row>
-    <row r="24" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="61"/>
       <c r="B24" s="104"/>
       <c r="C24" s="105" t="s">
@@ -8020,7 +8011,7 @@
       <c r="N24"/>
       <c r="P24" s="113"/>
     </row>
-    <row r="25" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="59"/>
       <c r="B25" s="104"/>
       <c r="C25" s="105" t="s">
@@ -8049,7 +8040,7 @@
       </c>
       <c r="U25" s="54"/>
     </row>
-    <row r="26" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="104"/>
       <c r="C26" s="105" t="s">
         <v>78</v>
@@ -8079,7 +8070,7 @@
       <c r="T26" s="121"/>
       <c r="U26" s="54"/>
     </row>
-    <row r="27" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:60" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="104"/>
       <c r="C27" s="105" t="s">
         <v>78</v>
@@ -8109,7 +8100,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:60" x14ac:dyDescent="0.2">
       <c r="B28" s="104"/>
       <c r="C28" s="105" t="s">
         <v>78</v>
@@ -8301,7 +8292,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="29" spans="1:60" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:60" s="61" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="56"/>
       <c r="B29" s="100"/>
       <c r="C29" s="101" t="s">
@@ -8497,7 +8488,7 @@
       <c r="BG29" s="56"/>
       <c r="BH29" s="56"/>
     </row>
-    <row r="30" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="56"/>
       <c r="B30" s="99"/>
       <c r="C30" s="67" t="s">
@@ -8694,7 +8685,7 @@
       <c r="BG30" s="56"/>
       <c r="BH30" s="56"/>
     </row>
-    <row r="31" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="56"/>
       <c r="B31" s="104"/>
       <c r="C31" s="67" t="s">
@@ -8890,7 +8881,7 @@
       <c r="BG31" s="56"/>
       <c r="BH31" s="56"/>
     </row>
-    <row r="32" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:60" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="56"/>
       <c r="B32" s="104"/>
       <c r="C32" s="67" t="s">
@@ -9083,7 +9074,7 @@
         <v>3.5169849357346781</v>
       </c>
     </row>
-    <row r="33" spans="1:57" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:57" s="61" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="56"/>
       <c r="B33" s="104"/>
       <c r="C33" s="67" t="s">
@@ -9150,7 +9141,7 @@
       <c r="BD33" s="56"/>
       <c r="BE33" s="56"/>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.2">
       <c r="B34" s="104"/>
       <c r="C34" s="67" t="s">
         <v>78</v>
@@ -9173,7 +9164,7 @@
         <v>MEUR20</v>
       </c>
     </row>
-    <row r="35" spans="1:57" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:57" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B35" s="100"/>
       <c r="C35" s="101" t="s">
         <v>78</v>
@@ -9238,7 +9229,7 @@
       <c r="BD35" s="41"/>
       <c r="BE35" s="41"/>
     </row>
-    <row r="36" spans="1:57" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:57" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B36" s="104"/>
       <c r="C36" s="67" t="s">
         <v>78</v>
@@ -9306,7 +9297,7 @@
       <c r="BD36" s="41"/>
       <c r="BE36" s="41"/>
     </row>
-    <row r="37" spans="1:57" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:57" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B37" s="104"/>
       <c r="C37" s="67" t="s">
         <v>78</v>
@@ -9371,7 +9362,7 @@
       <c r="BD37"/>
       <c r="BE37"/>
     </row>
-    <row r="38" spans="1:57" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:57" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B38" s="104"/>
       <c r="C38" s="67" t="s">
         <v>78</v>
@@ -9436,7 +9427,7 @@
       <c r="BD38"/>
       <c r="BE38"/>
     </row>
-    <row r="39" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A39" s="61"/>
       <c r="B39" s="104"/>
       <c r="C39" s="67" t="s">
@@ -9461,7 +9452,7 @@
       </c>
       <c r="Q39" s="118"/>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A40" s="61"/>
       <c r="B40" s="104"/>
       <c r="C40" s="67" t="s">
@@ -9492,7 +9483,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="41" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A41" s="61"/>
       <c r="B41" s="104"/>
       <c r="C41" s="105" t="s">
@@ -9519,7 +9510,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="42" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A42" s="61"/>
       <c r="B42" s="110"/>
       <c r="C42" s="111"/>
@@ -9534,29 +9525,29 @@
       <c r="L42" s="110"/>
       <c r="M42" s="110"/>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A43" s="61"/>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.2">
       <c r="C45" s="58"/>
       <c r="E45" s="63"/>
     </row>
-    <row r="46" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:57" x14ac:dyDescent="0.2">
       <c r="B46"/>
       <c r="C46" s="58"/>
       <c r="E46" s="63"/>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E49" s="60"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E50" s="60"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51"/>
       <c r="E51" s="60"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
@@ -9567,7 +9558,7 @@
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
@@ -9578,7 +9569,7 @@
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
@@ -9589,7 +9580,7 @@
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
@@ -9600,7 +9591,7 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
@@ -9611,7 +9602,7 @@
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
@@ -9622,7 +9613,7 @@
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B67"/>
       <c r="C67"/>
       <c r="D67"/>
@@ -9642,22 +9633,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="94" t="s">
         <v>37</v>
       </c>
@@ -9668,7 +9659,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="57" t="s">
         <v>38</v>
       </c>
@@ -9691,7 +9682,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="87" t="s">
         <v>979</v>
       </c>
@@ -9720,7 +9711,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="130" t="s">
         <v>980</v>
       </c>
@@ -9745,7 +9736,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="130" t="s">
         <v>981</v>
       </c>
@@ -9770,7 +9761,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="130" t="s">
         <v>982</v>
       </c>
@@ -9780,7 +9771,7 @@
       <c r="F7" s="133"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="130" t="s">
         <v>983</v>
       </c>
@@ -9790,7 +9781,7 @@
       <c r="F8" s="133"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="130" t="s">
         <v>984</v>
       </c>
@@ -9800,7 +9791,7 @@
       <c r="F9" s="133"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="130" t="s">
         <v>937</v>
       </c>
@@ -9810,7 +9801,7 @@
       <c r="F10" s="133"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="130" t="s">
         <v>985</v>
       </c>
@@ -9820,7 +9811,7 @@
       <c r="F11" s="133"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="130" t="s">
         <v>986</v>
       </c>
@@ -9830,7 +9821,7 @@
       <c r="F12" s="133"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="130" t="s">
         <v>987</v>
       </c>
@@ -9840,7 +9831,7 @@
       <c r="F13" s="133"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="2:15" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="130" t="s">
         <v>988</v>
       </c>
@@ -9850,7 +9841,7 @@
       <c r="F14" s="133"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="88" t="s">
         <v>71</v>
       </c>
@@ -9858,7 +9849,7 @@
       <c r="D15" s="56"/>
       <c r="E15" s="56"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="89" t="s">
         <v>72</v>
       </c>
@@ -9866,7 +9857,7 @@
       <c r="D16" s="56"/>
       <c r="E16" s="56"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="88" t="s">
         <v>73</v>
       </c>
@@ -9874,7 +9865,7 @@
       <c r="D17" s="56"/>
       <c r="E17" s="56"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="88" t="s">
         <v>74</v>
       </c>
@@ -9882,7 +9873,7 @@
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="89" t="s">
         <v>75</v>
       </c>
@@ -9890,7 +9881,7 @@
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="90" t="s">
         <v>946</v>
       </c>
@@ -9898,7 +9889,7 @@
       <c r="D20" s="56"/>
       <c r="E20" s="56"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="90" t="s">
         <v>944</v>
       </c>
@@ -9906,7 +9897,7 @@
       <c r="D21" s="56"/>
       <c r="E21" s="56"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="90" t="s">
         <v>945</v>
       </c>
@@ -9914,7 +9905,7 @@
       <c r="D22" s="56"/>
       <c r="E22" s="56"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="90" t="s">
         <v>962</v>
       </c>
@@ -9922,7 +9913,7 @@
       <c r="D23" s="56"/>
       <c r="E23" s="56"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="90" t="s">
         <v>963</v>
       </c>
@@ -9930,7 +9921,7 @@
       <c r="D24" s="56"/>
       <c r="E24" s="56"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="91" t="s">
         <v>964</v>
       </c>
@@ -9938,7 +9929,7 @@
       <c r="D25" s="56"/>
       <c r="E25" s="56"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="92" t="s">
         <v>938</v>
       </c>
@@ -9946,102 +9937,102 @@
       <c r="D26" s="56"/>
       <c r="E26" s="56"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="90" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="92" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="92" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="92" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31" s="91" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="92" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="90" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B34" s="90" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="90" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="90" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B37" s="91" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="93" t="s">
         <v>954</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="93" t="s">
         <v>955</v>
       </c>
       <c r="C39" s="41"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="93" t="s">
         <v>956</v>
       </c>
       <c r="C40" s="41"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="93"/>
       <c r="C41" s="41"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="93" t="s">
         <v>957</v>
       </c>
       <c r="C42" s="41"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B43" s="93" t="s">
         <v>990</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="93" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="93"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B46" s="93"/>
     </row>
   </sheetData>
@@ -10052,26 +10043,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z157"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>975</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.2">
       <c r="S5" s="41"/>
       <c r="T5" s="41"/>
       <c r="U5" s="41"/>
@@ -10081,7 +10072,7 @@
       <c r="Y5" s="41"/>
       <c r="Z5" s="41"/>
     </row>
-    <row r="6" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>973</v>
       </c>
@@ -10097,7 +10088,7 @@
       <c r="Y6" s="43"/>
       <c r="Z6" s="41"/>
     </row>
-    <row r="7" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.2">
       <c r="S7" s="41"/>
       <c r="T7" s="42"/>
       <c r="U7" s="42"/>
@@ -10107,7 +10098,7 @@
       <c r="Y7" s="42"/>
       <c r="Z7" s="42"/>
     </row>
-    <row r="8" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>2010</v>
       </c>
@@ -10132,7 +10123,7 @@
       <c r="Y8" s="125"/>
       <c r="Z8" s="125"/>
     </row>
-    <row r="9" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>2011</v>
       </c>
@@ -10157,7 +10148,7 @@
       <c r="Y9" s="125"/>
       <c r="Z9" s="125"/>
     </row>
-    <row r="10" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>2012</v>
       </c>
@@ -10182,7 +10173,7 @@
       <c r="Y10" s="126"/>
       <c r="Z10" s="126"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>2013</v>
       </c>
@@ -10206,7 +10197,7 @@
       <c r="Y11" s="125"/>
       <c r="Z11" s="125"/>
     </row>
-    <row r="12" spans="2:26" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B12">
         <v>2014</v>
       </c>
@@ -10231,7 +10222,7 @@
       <c r="Y12" s="47"/>
       <c r="Z12" s="47"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>2015</v>
       </c>
@@ -10247,7 +10238,7 @@
         <v>1.0675083333333333</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>2016</v>
       </c>
@@ -10263,7 +10254,7 @@
         <v>1.6065250000000002</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>2017</v>
       </c>
@@ -10279,7 +10270,7 @@
         <v>1.7234916666666666</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>2018</v>
       </c>
@@ -10295,7 +10286,7 @@
         <v>1.701225</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>2019</v>
       </c>
@@ -10311,7 +10302,7 @@
         <v>1.7024999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>2020</v>
       </c>
@@ -10327,7 +10318,7 @@
         <v>1.7035416666666665</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>966</v>
       </c>
@@ -10365,7 +10356,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>YEAR(B25)</f>
         <v>2021</v>
@@ -10407,7 +10398,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ref="A26:A89" si="2">YEAR(B26)</f>
         <v>2020</v>
@@ -10449,7 +10440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10491,7 +10482,7 @@
         <v>-6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10533,7 +10524,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10575,7 +10566,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10617,7 +10608,7 @@
         <v>-6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10659,7 +10650,7 @@
         <v>6.8999999999999999E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10701,7 +10692,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10743,7 +10734,7 @@
         <v>-8.3000000000000001E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10785,7 +10776,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10827,7 +10818,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10869,7 +10860,7 @@
         <v>1.6999999999999999E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" si="2"/>
         <v>2020</v>
@@ -10911,7 +10902,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -10953,7 +10944,7 @@
         <v>-1.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -10995,7 +10986,7 @@
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11037,7 +11028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11079,7 +11070,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11121,7 +11112,7 @@
         <v>-5.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11163,7 +11154,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11205,7 +11196,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11247,7 +11238,7 @@
         <v>-7.7000000000000002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11289,7 +11280,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11331,7 +11322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11373,7 +11364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" si="2"/>
         <v>2019</v>
@@ -11415,7 +11406,7 @@
         <v>-3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11457,7 +11448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11499,7 +11490,7 @@
         <v>-1.5E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11541,7 +11532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11583,7 +11574,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11625,7 +11616,7 @@
         <v>-1.5E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11667,7 +11658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11709,7 +11700,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11751,7 +11742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11793,7 +11784,7 @@
         <v>-1.5E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11835,7 +11826,7 @@
         <v>9.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11877,7 +11868,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="2"/>
         <v>2018</v>
@@ -11919,7 +11910,7 @@
         <v>-6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -11961,7 +11952,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12003,7 +11994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12045,7 +12036,7 @@
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12087,7 +12078,7 @@
         <v>-8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12129,7 +12120,7 @@
         <v>8.6E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12171,7 +12162,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12213,7 +12204,7 @@
         <v>-8.2000000000000007E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12255,7 +12246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12297,7 +12288,7 @@
         <v>-8.6999999999999994E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12339,7 +12330,7 @@
         <v>-2.8299999999999999E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12381,7 +12372,7 @@
         <v>-9.4E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="2"/>
         <v>2017</v>
@@ -12423,7 +12414,7 @@
         <v>8.1299999999999997E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12465,7 +12456,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12507,7 +12498,7 @@
         <v>6.7699999999999996E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12549,7 +12540,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A77">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12591,7 +12582,7 @@
         <v>-6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12633,7 +12624,7 @@
         <v>2.8899999999999999E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12675,7 +12666,7 @@
         <v>2.9700000000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12717,7 +12708,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12759,7 +12750,7 @@
         <v>-1.43E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12801,7 +12792,7 @@
         <v>-1.9400000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12843,7 +12834,7 @@
         <v>-1.5100000000000001E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12885,7 +12876,7 @@
         <v>-2.3E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>2016</v>
@@ -12927,7 +12918,7 @@
         <v>2.64E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>2015</v>
@@ -12969,7 +12960,7 @@
         <v>0.49259999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="2"/>
         <v>2015</v>
@@ -13011,7 +13002,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>2015</v>
@@ -13053,7 +13044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="2"/>
         <v>2015</v>
@@ -13095,7 +13086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" ref="A90:A153" si="3">YEAR(B90)</f>
         <v>2015</v>
@@ -13137,7 +13128,7 @@
         <v>-6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13179,7 +13170,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13221,7 +13212,7 @@
         <v>-8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13263,7 +13254,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13305,7 +13296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13347,7 +13338,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13389,7 +13380,7 @@
         <v>0.33739999999999998</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="3"/>
         <v>2015</v>
@@ -13431,7 +13422,7 @@
         <v>-2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13473,7 +13464,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13515,7 +13506,7 @@
         <v>-1E-3</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13557,7 +13548,7 @@
         <v>8.0000000000000004E-4</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13599,7 +13590,7 @@
         <v>-2.3E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13641,7 +13632,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13683,7 +13674,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13725,7 +13716,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13767,7 +13758,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13809,7 +13800,7 @@
         <v>-1.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13851,7 +13842,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A108">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13893,7 +13884,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A109">
         <f t="shared" si="3"/>
         <v>2014</v>
@@ -13935,7 +13926,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A110">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -13977,7 +13968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14019,7 +14010,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14061,7 +14052,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14103,7 +14094,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14145,7 +14136,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14187,7 +14178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14229,7 +14220,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14271,7 +14262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14313,7 +14304,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14355,7 +14346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14397,7 +14388,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="3"/>
         <v>2013</v>
@@ -14439,7 +14430,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14481,7 +14472,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14523,7 +14514,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14565,7 +14556,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14607,7 +14598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14649,7 +14640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14691,7 +14682,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14733,7 +14724,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14775,7 +14766,7 @@
         <v>-5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14817,7 +14808,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14859,7 +14850,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14901,7 +14892,7 @@
         <v>-2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="3"/>
         <v>2012</v>
@@ -14943,7 +14934,7 @@
         <v>-1E-4</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -14985,7 +14976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15027,7 +15018,7 @@
         <v>-4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15069,7 +15060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15111,7 +15102,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15153,7 +15144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15195,7 +15186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15237,7 +15228,7 @@
         <v>-1.3100000000000001E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15279,7 +15270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15321,7 +15312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15363,7 +15354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15405,7 +15396,7 @@
         <v>-1.4E-3</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="3"/>
         <v>2011</v>
@@ -15447,7 +15438,7 @@
         <v>-4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15489,7 +15480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15531,7 +15522,7 @@
         <v>-1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15573,7 +15564,7 @@
         <v>-2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15615,7 +15606,7 @@
         <v>-8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15657,7 +15648,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15699,7 +15690,7 @@
         <v>-5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15741,7 +15732,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="3"/>
         <v>2010</v>
@@ -15783,7 +15774,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" ref="A154:A157" si="4">YEAR(B154)</f>
         <v>2010</v>
@@ -15825,7 +15816,7 @@
         <v>-2.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="4"/>
         <v>2010</v>
@@ -15867,7 +15858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="4"/>
         <v>2010</v>
@@ -15909,7 +15900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="4"/>
         <v>2010</v>
@@ -15957,24 +15948,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AV54"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="5" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="42" t="s">
         <v>88</v>
       </c>
@@ -15985,7 +15976,7 @@
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
     </row>
-    <row r="6" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="31"/>
       <c r="C6" s="44">
         <v>2010</v>
@@ -16009,7 +16000,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:48" ht="13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="45"/>
       <c r="B7" s="46" t="s">
         <v>89</v>
@@ -16043,7 +16034,7 @@
         <v>7.8615548740460981E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="45"/>
       <c r="B8" s="48" t="s">
         <v>90</v>
@@ -16077,7 +16068,7 @@
         <v>0.80182435242407102</v>
       </c>
     </row>
-    <row r="9" spans="1:48" ht="13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="45"/>
       <c r="B9" s="46" t="s">
         <v>91</v>
@@ -16111,7 +16102,7 @@
         <v>1.0559216083797939E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="B10" s="46" t="s">
         <v>92</v>
       </c>
@@ -16144,7 +16135,7 @@
         <v>0.10769671819564115</v>
       </c>
     </row>
-    <row r="11" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45"/>
       <c r="B11" s="46" t="s">
         <v>93</v>
@@ -16178,7 +16169,7 @@
         <v>0.13431460128400066</v>
       </c>
     </row>
-    <row r="12" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:48" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="45"/>
       <c r="B12" s="46"/>
       <c r="C12" s="50"/>
@@ -16188,71 +16179,71 @@
       <c r="G12" s="50"/>
       <c r="H12" s="50"/>
     </row>
-    <row r="13" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:48" ht="13" x14ac:dyDescent="0.3">
-      <c r="A15" s="152" t="s">
+    <row r="14" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A15" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="152"/>
-      <c r="C15" s="152"/>
-      <c r="D15" s="152"/>
-      <c r="E15" s="152"/>
-      <c r="F15" s="152"/>
-      <c r="H15" s="152" t="s">
+      <c r="B15" s="153"/>
+      <c r="C15" s="153"/>
+      <c r="D15" s="153"/>
+      <c r="E15" s="153"/>
+      <c r="F15" s="153"/>
+      <c r="H15" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="152"/>
-      <c r="J15" s="152"/>
-      <c r="K15" s="152"/>
-      <c r="L15" s="152"/>
-      <c r="M15" s="152"/>
-      <c r="O15" s="152" t="s">
+      <c r="I15" s="153"/>
+      <c r="J15" s="153"/>
+      <c r="K15" s="153"/>
+      <c r="L15" s="153"/>
+      <c r="M15" s="153"/>
+      <c r="O15" s="153" t="s">
         <v>97</v>
       </c>
-      <c r="P15" s="152"/>
-      <c r="Q15" s="152"/>
-      <c r="R15" s="152"/>
-      <c r="S15" s="152"/>
-      <c r="T15" s="152"/>
-      <c r="V15" s="152" t="s">
+      <c r="P15" s="153"/>
+      <c r="Q15" s="153"/>
+      <c r="R15" s="153"/>
+      <c r="S15" s="153"/>
+      <c r="T15" s="153"/>
+      <c r="V15" s="153" t="s">
         <v>98</v>
       </c>
-      <c r="W15" s="152"/>
-      <c r="X15" s="152"/>
-      <c r="Y15" s="152"/>
-      <c r="Z15" s="152"/>
-      <c r="AA15" s="152"/>
-      <c r="AC15" s="152" t="s">
+      <c r="W15" s="153"/>
+      <c r="X15" s="153"/>
+      <c r="Y15" s="153"/>
+      <c r="Z15" s="153"/>
+      <c r="AA15" s="153"/>
+      <c r="AC15" s="153" t="s">
         <v>99</v>
       </c>
-      <c r="AD15" s="152"/>
-      <c r="AE15" s="152"/>
-      <c r="AF15" s="152"/>
-      <c r="AG15" s="152"/>
-      <c r="AH15" s="152"/>
-      <c r="AJ15" s="152" t="s">
+      <c r="AD15" s="153"/>
+      <c r="AE15" s="153"/>
+      <c r="AF15" s="153"/>
+      <c r="AG15" s="153"/>
+      <c r="AH15" s="153"/>
+      <c r="AJ15" s="153" t="s">
         <v>100</v>
       </c>
-      <c r="AK15" s="152"/>
-      <c r="AL15" s="152"/>
-      <c r="AM15" s="152"/>
-      <c r="AN15" s="152"/>
-      <c r="AO15" s="152"/>
-      <c r="AQ15" s="151" t="s">
+      <c r="AK15" s="153"/>
+      <c r="AL15" s="153"/>
+      <c r="AM15" s="153"/>
+      <c r="AN15" s="153"/>
+      <c r="AO15" s="153"/>
+      <c r="AQ15" s="152" t="s">
         <v>824</v>
       </c>
-      <c r="AR15" s="151"/>
-      <c r="AS15" s="151"/>
-      <c r="AT15" s="151"/>
-      <c r="AU15" s="151"/>
-      <c r="AV15" s="151"/>
-    </row>
-    <row r="16" spans="1:48" ht="13" x14ac:dyDescent="0.3">
+      <c r="AR15" s="152"/>
+      <c r="AS15" s="152"/>
+      <c r="AT15" s="152"/>
+      <c r="AU15" s="152"/>
+      <c r="AV15" s="152"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
         <v>101</v>
       </c>
@@ -16380,7 +16371,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -16508,7 +16499,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -16636,7 +16627,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -16764,7 +16755,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>100</v>
       </c>
@@ -16892,7 +16883,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -17020,7 +17011,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>100</v>
       </c>
@@ -17148,7 +17139,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A23" s="34">
         <v>100</v>
       </c>
@@ -17276,7 +17267,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="24" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -17404,7 +17395,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="25" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A25" s="52">
         <v>1</v>
       </c>
@@ -17532,7 +17523,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -17660,7 +17651,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -17788,7 +17779,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="28" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>100</v>
       </c>
@@ -17916,7 +17907,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="29" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>100</v>
       </c>
@@ -18044,7 +18035,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="30" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>100</v>
       </c>
@@ -18172,7 +18163,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="31" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>100</v>
       </c>
@@ -18300,7 +18291,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="32" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>100</v>
       </c>
@@ -18428,7 +18419,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="33" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>100</v>
       </c>
@@ -18556,7 +18547,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="34" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -18684,7 +18675,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="35" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -18812,7 +18803,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="36" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -18940,7 +18931,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="37" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -19068,7 +19059,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="38" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A38" s="7">
         <v>100</v>
       </c>
@@ -19196,7 +19187,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="39" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -19324,7 +19315,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="40" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -19452,7 +19443,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="41" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>100</v>
       </c>
@@ -19580,7 +19571,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="42" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -19708,7 +19699,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="43" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -19836,7 +19827,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="44" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -19964,7 +19955,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="45" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -20056,7 +20047,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="46" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -20130,7 +20121,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="47" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -20150,9 +20141,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="48" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50">
         <v>1</v>
       </c>
@@ -20165,7 +20156,7 @@
         <v>0.92999462253555654</v>
       </c>
     </row>
-    <row r="51" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="40" t="s">
         <v>561</v>
       </c>
@@ -20176,12 +20167,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="40"/>
       <c r="C53" s="40"/>
     </row>
-    <row r="54" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D54" s="40"/>
     </row>
   </sheetData>

</xml_diff>